<commit_message>
Create template for coding multiple table same level
</commit_message>
<xml_diff>
--- a/template-non-multi.xlsx
+++ b/template-non-multi.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5175" yWindow="1800" windowWidth="28035" windowHeight="17445" activeTab="1"/>
+    <workbookView xWindow="5175" yWindow="1800" windowWidth="28035" windowHeight="17445" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="config" sheetId="2" r:id="rId2"/>
+    <sheet name="data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913" iterate="1"/>
   <extLst>
@@ -159,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="72">
   <si>
     <t>range_1</t>
   </si>
@@ -237,13 +238,151 @@
   </si>
   <si>
     <t>A8</t>
+  </si>
+  <si>
+    <t>index_table_excel</t>
+  </si>
+  <si>
+    <t>ROW_NUM</t>
+  </si>
+  <si>
+    <t>ACCOUNT_CODE</t>
+  </si>
+  <si>
+    <t>CUSTOMER_CODE</t>
+  </si>
+  <si>
+    <t>CUSTOMER_NAME</t>
+  </si>
+  <si>
+    <t>CUSTOMER_ADDRESS</t>
+  </si>
+  <si>
+    <t>SHARE_CODE</t>
+  </si>
+  <si>
+    <t>SHARE_VOLUME</t>
+  </si>
+  <si>
+    <t>CASH_BALANCE</t>
+  </si>
+  <si>
+    <t>C001</t>
+  </si>
+  <si>
+    <t>Nguyen Van C001</t>
+  </si>
+  <si>
+    <t>SN 01, Hai Ba Trung, Ha Noi</t>
+  </si>
+  <si>
+    <t>FPT</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>MBS</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>AGM</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>C0011</t>
+  </si>
+  <si>
+    <t>C0016</t>
+  </si>
+  <si>
+    <t>362500000</t>
+  </si>
+  <si>
+    <t>128300000</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>C002</t>
+  </si>
+  <si>
+    <t>Nguyen Van C002</t>
+  </si>
+  <si>
+    <t>SN 02, Hai Ba Trung, Ha Noi</t>
+  </si>
+  <si>
+    <t>1700</t>
+  </si>
+  <si>
+    <t>8000</t>
+  </si>
+  <si>
+    <t>4500</t>
+  </si>
+  <si>
+    <t>992000000</t>
+  </si>
+  <si>
+    <t>144120000</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>C003</t>
+  </si>
+  <si>
+    <t>Nguyen Van C003</t>
+  </si>
+  <si>
+    <t>SN 03, Hai Ba Trung, Ha Noi</t>
+  </si>
+  <si>
+    <t>7700</t>
+  </si>
+  <si>
+    <t>8100</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>512000000</t>
+  </si>
+  <si>
+    <t>523600000</t>
+  </si>
+  <si>
+    <t>INDEX_TABLE_EXCEL</t>
+  </si>
+  <si>
+    <t>TABLE_01</t>
+  </si>
+  <si>
+    <t>TABLE_02</t>
+  </si>
+  <si>
+    <t>ROW_NUM_SHARE</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ROW_NUM_CASH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -303,8 +442,22 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +473,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -454,6 +655,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15.75"/>
@@ -912,7 +1125,7 @@
     <col min="1" max="1" width="17.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.44140625" style="2"/>
     <col min="4" max="4" width="16.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="2"/>
+    <col min="5" max="5" width="20.44140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.109375" style="2" bestFit="1" customWidth="1"/>
@@ -921,7 +1134,7 @@
     <col min="11" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -929,7 +1142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -937,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -947,8 +1160,11 @@
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -961,8 +1177,9 @@
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -973,6 +1190,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -980,4 +1198,504 @@
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="6.88671875" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="26"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="25" customFormat="1" ht="18" customHeight="1">
+      <c r="A1" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="18" customHeight="1">
+      <c r="A2" s="28">
+        <v>1</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18" customHeight="1">
+      <c r="A3" s="28">
+        <v>1</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" customHeight="1">
+      <c r="A4" s="28">
+        <v>1</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" customHeight="1">
+      <c r="A5" s="28">
+        <v>1</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" customHeight="1">
+      <c r="A6" s="28">
+        <v>1</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" customHeight="1">
+      <c r="A7" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" customHeight="1">
+      <c r="A8" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" customHeight="1">
+      <c r="A9" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18" customHeight="1">
+      <c r="A10" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" customHeight="1">
+      <c r="A11" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18" customHeight="1">
+      <c r="A12" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" customHeight="1">
+      <c r="A13" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18" customHeight="1">
+      <c r="A14" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="18" customHeight="1">
+      <c r="A15" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="18" customHeight="1">
+      <c r="A16" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>